<commit_message>
This message is added with the help of amend + temp
</commit_message>
<xml_diff>
--- a/myExcel.xlsx
+++ b/myExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Temp\Git &amp; GitHub\Complete GitHub\Tutorial2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B77313-25C2-4093-A268-5CF8C1AA44E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2412917F-1AA8-4AE0-B512-C6AA22DCF6F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>erer</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>fddfdf</t>
+  </si>
+  <si>
+    <t>sdsdsd</t>
   </si>
 </sst>
 </file>
@@ -360,35 +363,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="K11" sqref="J11:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -396,9 +399,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K11" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>